<commit_message>
Updated code to reflect current version of the paper
</commit_message>
<xml_diff>
--- a/Python/BCData1.xlsx
+++ b/Python/BCData1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klp4/Dropbox/Papers/5 in progress/sleep-simulation/econsleep-bitbucket/Drafts/Business Cycle/Python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klp4/Dropbox/Papers/5 in progress/sleep-simulation/econ sleep project/Drafts/Business Cycle/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="460" windowWidth="23840" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="1760" yWindow="460" windowWidth="10000" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="del">[1]Data1!$E$18</definedName>
   </definedNames>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>K</t>
   </si>
@@ -55,11 +55,24 @@
   <si>
     <t>ConsPC</t>
   </si>
+  <si>
+    <t>Inv</t>
+  </si>
+  <si>
+    <t>Cons</t>
+  </si>
+  <si>
+    <t>Govt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="12"/>
@@ -89,9 +102,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,15 +422,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K56" sqref="K56"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,8 +452,17 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>40455.279893908453</v>
       </c>
@@ -446,22 +470,31 @@
         <v>13031.2</v>
       </c>
       <c r="C2">
-        <v>519.2247141051937</v>
+        <v>510.12106774299684</v>
       </c>
       <c r="D2">
-        <v>182.92694278260149</v>
+        <v>226.69082826551113</v>
       </c>
       <c r="E2">
-        <v>254.74160114323234</v>
+        <v>221.84085937690963</v>
       </c>
       <c r="F2">
-        <v>474.26080404694176</v>
+        <v>452.25322298482513</v>
       </c>
       <c r="G2" s="1">
         <v>30084</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="2">
+        <v>2239.5</v>
+      </c>
+      <c r="I2" s="3">
+        <v>8712.527</v>
+      </c>
+      <c r="J2" s="3">
+        <v>2728.2910000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>40663.291745922383</v>
       </c>
@@ -469,22 +502,31 @@
         <v>13152.1</v>
       </c>
       <c r="C3">
-        <v>521.05012520574246</v>
+        <v>513.43857338989949</v>
       </c>
       <c r="D3">
-        <v>174.5617020084533</v>
+        <v>221.59533719685862</v>
       </c>
       <c r="E3">
-        <v>250.85574495528749</v>
+        <v>218.05313865846793</v>
       </c>
       <c r="F3">
-        <v>484.95995294434618</v>
+        <v>463.11795696465737</v>
       </c>
       <c r="G3" s="1">
         <v>30351</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" s="2">
+        <v>2251.3000000000002</v>
+      </c>
+      <c r="I3" s="3">
+        <v>8809.5069999999996</v>
+      </c>
+      <c r="J3" s="3">
+        <v>2771.221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>40872.444397622778</v>
       </c>
@@ -492,22 +534,31 @@
         <v>13372.4</v>
       </c>
       <c r="C4">
-        <v>525.76016851039162</v>
+        <v>516.91933187679695</v>
       </c>
       <c r="D4">
-        <v>172.38974128087298</v>
+        <v>221.17916953270912</v>
       </c>
       <c r="E4">
-        <v>258.57457571374334</v>
+        <v>220.86446962268536</v>
       </c>
       <c r="F4">
-        <v>476.4668059764382</v>
+        <v>448.22509010116983</v>
       </c>
       <c r="G4" s="1">
         <v>30722</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="2">
+        <v>2330.9</v>
+      </c>
+      <c r="I4" s="3">
+        <v>8939.3870000000006</v>
+      </c>
+      <c r="J4" s="3">
+        <v>2771.2379999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>41099.677926809869</v>
       </c>
@@ -515,22 +566,31 @@
         <v>13528.7</v>
       </c>
       <c r="C5">
-        <v>527.98082881774462</v>
+        <v>517.61735628642464</v>
       </c>
       <c r="D5">
-        <v>175.61758038386537</v>
+        <v>227.19583868845751</v>
       </c>
       <c r="E5">
-        <v>242.29809068374294</v>
+        <v>205.05646644268091</v>
       </c>
       <c r="F5">
-        <v>480.98067452913949</v>
+        <v>456.18451951026543</v>
       </c>
       <c r="G5" s="1">
         <v>30887</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" s="2">
+        <v>2413.1</v>
+      </c>
+      <c r="I5" s="3">
+        <v>9008.8150000000005</v>
+      </c>
+      <c r="J5" s="3">
+        <v>2786.3229999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>41345.485073553995</v>
       </c>
@@ -538,22 +598,31 @@
         <v>13606.5</v>
       </c>
       <c r="C6">
-        <v>523.46928745189427</v>
+        <v>511.85791922996123</v>
       </c>
       <c r="D6">
-        <v>175.87774440031578</v>
+        <v>227.07271491489553</v>
       </c>
       <c r="E6">
-        <v>250.59337263960055</v>
+        <v>216.48548986756794</v>
       </c>
       <c r="F6">
-        <v>482.59498741798791</v>
+        <v>457.32795507961941</v>
       </c>
       <c r="G6" s="1">
         <v>31127</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="2">
+        <v>2414.5</v>
+      </c>
+      <c r="I6" s="3">
+        <v>9096.4150000000009</v>
+      </c>
+      <c r="J6" s="3">
+        <v>2793.9349999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>41589.504292277903</v>
       </c>
@@ -561,22 +630,31 @@
         <v>13706.2</v>
       </c>
       <c r="C7">
-        <v>519.16853521282064</v>
+        <v>511.84162241102518</v>
       </c>
       <c r="D7">
-        <v>169.90101359343885</v>
+        <v>219.53132850845631</v>
       </c>
       <c r="E7">
-        <v>249.83018838794459</v>
+        <v>219.89980301772525</v>
       </c>
       <c r="F7">
-        <v>494.57596047892071</v>
+        <v>469.47239259219469</v>
       </c>
       <c r="G7" s="1">
         <v>31261</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7" s="2">
+        <v>2500.9</v>
+      </c>
+      <c r="I7" s="3">
+        <v>9155.4680000000008</v>
+      </c>
+      <c r="J7" s="3">
+        <v>2809.9229999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>41853.001133633654</v>
       </c>
@@ -584,22 +662,31 @@
         <v>13830.8</v>
       </c>
       <c r="C8">
-        <v>518.3707440419812</v>
+        <v>507.77840534274696</v>
       </c>
       <c r="D8">
-        <v>190.32233278664546</v>
+        <v>238.93374146036186</v>
       </c>
       <c r="E8">
-        <v>247.16304051124206</v>
+        <v>211.8943064394517</v>
       </c>
       <c r="F8">
-        <v>477.53018153492496</v>
+        <v>455.67237237564268</v>
       </c>
       <c r="G8" s="1">
         <v>31481</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8" s="2">
+        <v>2539.4</v>
+      </c>
+      <c r="I8" s="3">
+        <v>9243.0020000000004</v>
+      </c>
+      <c r="J8" s="3">
+        <v>2820.6640000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>42123.831189384982</v>
       </c>
@@ -607,22 +694,31 @@
         <v>13950.4</v>
       </c>
       <c r="C9">
-        <v>527.23187843618871</v>
+        <v>521.89930371334253</v>
       </c>
       <c r="D9">
-        <v>170.62542488152852</v>
+        <v>216.33686031581584</v>
       </c>
       <c r="E9">
-        <v>248.15590471780058</v>
+        <v>210.48920427495585</v>
       </c>
       <c r="F9">
-        <v>484.56112390975727</v>
+        <v>455.12220066215457</v>
       </c>
       <c r="G9" s="1">
         <v>31725</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9" s="2">
+        <v>2590.6</v>
+      </c>
+      <c r="I9" s="3">
+        <v>9337.8369999999995</v>
+      </c>
+      <c r="J9" s="3">
+        <v>2808.2289999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>42405.105678292239</v>
       </c>
@@ -630,22 +726,31 @@
         <v>14099.1</v>
       </c>
       <c r="C10">
-        <v>522.27846090819537</v>
+        <v>512.69214430689192</v>
       </c>
       <c r="D10">
-        <v>174.48750484328022</v>
+        <v>225.67486001791701</v>
       </c>
       <c r="E10">
-        <v>259.12021558839854</v>
+        <v>222.15164405364462</v>
       </c>
       <c r="F10">
-        <v>474.81444958661098</v>
+        <v>452.03674957235717</v>
       </c>
       <c r="G10" s="1">
         <v>31900</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10" s="2">
+        <v>2664.4</v>
+      </c>
+      <c r="I10" s="3">
+        <v>9409.2219999999998</v>
+      </c>
+      <c r="J10" s="3">
+        <v>2814.0909999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>42702.383759032877</v>
       </c>
@@ -653,22 +758,31 @@
         <v>14172.7</v>
       </c>
       <c r="C11">
-        <v>526.77633151469945</v>
+        <v>520.28436691078605</v>
       </c>
       <c r="D11">
-        <v>175.46053276966668</v>
+        <v>222.16488705631616</v>
       </c>
       <c r="E11">
-        <v>243.52451801097402</v>
+        <v>213.06864066213052</v>
       </c>
       <c r="F11">
-        <v>482.69761215151345</v>
+        <v>461.13134842878401</v>
       </c>
       <c r="G11" s="1">
         <v>32178</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" s="2">
+        <v>2630.5</v>
+      </c>
+      <c r="I11" s="3">
+        <v>9511.4509999999991</v>
+      </c>
+      <c r="J11" s="3">
+        <v>2818.942</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>42988.60123904128</v>
       </c>
@@ -676,22 +790,31 @@
         <v>14291.8</v>
       </c>
       <c r="C12">
-        <v>527.60192731775919</v>
+        <v>519.16955815073777</v>
       </c>
       <c r="D12">
-        <v>181.11264440962276</v>
+        <v>225.53311203755669</v>
       </c>
       <c r="E12">
-        <v>251.71151885396978</v>
+        <v>213.61410848492568</v>
       </c>
       <c r="F12">
-        <v>468.99559802663691</v>
+        <v>447.98125476844103</v>
       </c>
       <c r="G12" s="1">
         <v>32345</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12" s="2">
+        <v>2657.9</v>
+      </c>
+      <c r="I12" s="3">
+        <v>9585.2330000000002</v>
+      </c>
+      <c r="J12" s="3">
+        <v>2840.97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>43279.179318808514</v>
       </c>
@@ -699,22 +822,31 @@
         <v>14373.4</v>
       </c>
       <c r="C13">
-        <v>526.52234752812092</v>
+        <v>520.12517963981054</v>
       </c>
       <c r="D13">
-        <v>179.85758624444478</v>
+        <v>224.81297668898128</v>
       </c>
       <c r="E13">
-        <v>240.83395416507977</v>
+        <v>201.04371859272749</v>
       </c>
       <c r="F13">
-        <v>485.19393855665669</v>
+        <v>468.71480849572708</v>
       </c>
       <c r="G13" s="1">
         <v>32386</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13" s="2">
+        <v>2737.6</v>
+      </c>
+      <c r="I13" s="3">
+        <v>9621.3389999999999</v>
+      </c>
+      <c r="J13" s="3">
+        <v>2830.703</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>43587.155071656969</v>
       </c>
@@ -722,22 +854,31 @@
         <v>14546.1</v>
       </c>
       <c r="C14">
-        <v>520.1230691992763</v>
+        <v>510.48847236593247</v>
       </c>
       <c r="D14">
-        <v>183.47696900019011</v>
+        <v>239.43178998239236</v>
       </c>
       <c r="E14">
-        <v>249.25655216788664</v>
+        <v>205.79887662409874</v>
       </c>
       <c r="F14">
-        <v>473.48117086723278</v>
+        <v>450.16579454490352</v>
       </c>
       <c r="G14" s="1">
         <v>32677</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14" s="2">
+        <v>2773.8</v>
+      </c>
+      <c r="I14" s="3">
+        <v>9729.2250000000004</v>
+      </c>
+      <c r="J14" s="3">
+        <v>2853.4960000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>43901.502179883879</v>
       </c>
@@ -745,22 +886,31 @@
         <v>14589.6</v>
       </c>
       <c r="C15">
-        <v>523.91263371771424</v>
+        <v>515.97907006981234</v>
       </c>
       <c r="D15">
-        <v>180.52558224268284</v>
+        <v>229.8952623410392</v>
       </c>
       <c r="E15">
-        <v>242.90549430090948</v>
+        <v>203.83696318586155</v>
       </c>
       <c r="F15">
-        <v>480.41852927270918</v>
+        <v>458.55661647787224</v>
       </c>
       <c r="G15" s="1">
         <v>32777</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H15" s="2">
+        <v>2755.7</v>
+      </c>
+      <c r="I15" s="3">
+        <v>9781.0249999999996</v>
+      </c>
+      <c r="J15" s="3">
+        <v>2864.1219999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>44208.590228098081</v>
       </c>
@@ -768,22 +918,31 @@
         <v>14602.6</v>
       </c>
       <c r="C16">
-        <v>534.88632283242828</v>
+        <v>527.81549911192951</v>
       </c>
       <c r="D16">
-        <v>177.0030410922185</v>
+        <v>223.94473789753638</v>
       </c>
       <c r="E16">
-        <v>251.87213563583538</v>
+        <v>215.10260929297391</v>
       </c>
       <c r="F16">
-        <v>465.81144987252776</v>
+        <v>442.43399782727988</v>
       </c>
       <c r="G16" s="1">
         <v>32884</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16" s="2">
+        <v>2727.6</v>
+      </c>
+      <c r="I16" s="3">
+        <v>9838.1059999999998</v>
+      </c>
+      <c r="J16" s="3">
+        <v>2870.4259999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>44505.982352575338</v>
       </c>
@@ -791,22 +950,31 @@
         <v>14716.9</v>
       </c>
       <c r="C17">
-        <v>526.98670401150184</v>
+        <v>516.19150319116011</v>
       </c>
       <c r="D17">
-        <v>184.90894604964953</v>
+        <v>233.40977462306168</v>
       </c>
       <c r="E17">
-        <v>243.54849959266241</v>
+        <v>204.97995749688187</v>
       </c>
       <c r="F17">
-        <v>475.19939670082113</v>
+        <v>454.84538427979055</v>
       </c>
       <c r="G17" s="1">
         <v>33134</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17" s="2">
+        <v>2663</v>
+      </c>
+      <c r="I17" s="3">
+        <v>9938.4089999999997</v>
+      </c>
+      <c r="J17" s="3">
+        <v>2889.085</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>44784.637884415504</v>
       </c>
@@ -814,22 +982,31 @@
         <v>14726</v>
       </c>
       <c r="C18">
-        <v>524.30728709990626</v>
+        <v>513.67032777272698</v>
       </c>
       <c r="D18">
-        <v>186.02192696407604</v>
+        <v>227.32359528447219</v>
       </c>
       <c r="E18">
-        <v>244.11927591431882</v>
+        <v>213.54242282080367</v>
       </c>
       <c r="F18">
-        <v>474.99690913945631</v>
+        <v>454.39308981840111</v>
       </c>
       <c r="G18" s="1">
         <v>33235</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18" s="2">
+        <v>2638.5</v>
+      </c>
+      <c r="I18" s="3">
+        <v>9990.6569999999992</v>
+      </c>
+      <c r="J18" s="3">
+        <v>2882.7440000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>45054.744786685093</v>
       </c>
@@ -837,22 +1014,31 @@
         <v>14838.7</v>
       </c>
       <c r="C19">
-        <v>525.10384315790111</v>
+        <v>518.47950119103848</v>
       </c>
       <c r="D19">
-        <v>182.12605014431026</v>
+        <v>221.19025506861149</v>
       </c>
       <c r="E19">
-        <v>237.12893517807612</v>
+        <v>207.57204990639778</v>
       </c>
       <c r="F19">
-        <v>485.63494702188643</v>
+        <v>468.52706587986</v>
       </c>
       <c r="G19" s="1">
         <v>33273</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="H19" s="2">
+        <v>2674.7</v>
+      </c>
+      <c r="I19" s="3">
+        <v>10024.603999999999</v>
+      </c>
+      <c r="J19" s="3">
+        <v>2907.0340000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>45331.552411797915</v>
       </c>
@@ -860,22 +1046,31 @@
         <v>14938.5</v>
       </c>
       <c r="C20">
-        <v>523.50375595500873</v>
+        <v>510.51401672764575</v>
       </c>
       <c r="D20">
-        <v>184.82971233965898</v>
+        <v>234.34780989720394</v>
       </c>
       <c r="E20">
-        <v>244.80291223775666</v>
+        <v>211.05723084534714</v>
       </c>
       <c r="F20">
-        <v>474.0862617786305</v>
+        <v>450.78332829935869</v>
       </c>
       <c r="G20" s="1">
         <v>33335</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20" s="2">
+        <v>2658.1</v>
+      </c>
+      <c r="I20" s="3">
+        <v>10069.157999999999</v>
+      </c>
+      <c r="J20" s="3">
+        <v>2928.0479999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>45601.802479661987</v>
       </c>
@@ -883,22 +1078,31 @@
         <v>14991.8</v>
       </c>
       <c r="C21">
-        <v>528.18111673610042</v>
+        <v>518.37654311339486</v>
       </c>
       <c r="D21">
-        <v>183.30214537868386</v>
+        <v>234.48254543018658</v>
       </c>
       <c r="E21">
-        <v>239.40276658297591</v>
+        <v>203.70016842933245</v>
       </c>
       <c r="F21">
-        <v>478.83984035260914</v>
+        <v>452.09922906187137</v>
       </c>
       <c r="G21" s="1">
         <v>33292</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H21" s="2">
+        <v>2605.1999999999998</v>
+      </c>
+      <c r="I21" s="3">
+        <v>10081.798000000001</v>
+      </c>
+      <c r="J21" s="3">
+        <v>2939.81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>45856.477025174674</v>
       </c>
@@ -906,22 +1110,31 @@
         <v>14889.5</v>
       </c>
       <c r="C22">
-        <v>522.10706594630994</v>
+        <v>511.86409187693937</v>
       </c>
       <c r="D22">
-        <v>178.30822568867637</v>
+        <v>228.78270672086231</v>
       </c>
       <c r="E22">
-        <v>241.26538563065714</v>
+        <v>204.48046021597264</v>
       </c>
       <c r="F22">
-        <v>487.69243453997944</v>
+        <v>464.69664752687913</v>
       </c>
       <c r="G22" s="1">
         <v>33150</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22" s="2">
+        <v>2517.5</v>
+      </c>
+      <c r="I22" s="3">
+        <v>10060.966</v>
+      </c>
+      <c r="J22" s="3">
+        <v>2951.9879999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>46087.011517731822</v>
       </c>
@@ -929,22 +1142,31 @@
         <v>14963.4</v>
       </c>
       <c r="C23">
-        <v>526.60649321049095</v>
+        <v>517.57193368955154</v>
       </c>
       <c r="D23">
-        <v>175.77822259867133</v>
+        <v>219.47670561242771</v>
       </c>
       <c r="E23">
-        <v>232.22541951705892</v>
+        <v>203.10959324382134</v>
       </c>
       <c r="F23">
-        <v>493.23054629880971</v>
+        <v>471.95887904264271</v>
       </c>
       <c r="G23" s="1">
         <v>33134</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23" s="2">
+        <v>2472.6</v>
+      </c>
+      <c r="I23" s="3">
+        <v>10077.94</v>
+      </c>
+      <c r="J23" s="3">
+        <v>2974.9810000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>46304.315917443659</v>
       </c>
@@ -952,22 +1174,31 @@
         <v>14891.6</v>
       </c>
       <c r="C24">
-        <v>528.60807642028726</v>
+        <v>511.68226714642532</v>
       </c>
       <c r="D24">
-        <v>175.39523472019192</v>
+        <v>234.36471415805806</v>
       </c>
       <c r="E24">
-        <v>246.10997492247481</v>
+        <v>208.13388048242271</v>
       </c>
       <c r="F24">
-        <v>478.96179649652788</v>
+        <v>453.02603810755477</v>
       </c>
       <c r="G24" s="1">
         <v>32814</v>
       </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24" s="2">
+        <v>2403.8000000000002</v>
+      </c>
+      <c r="I24" s="3">
+        <v>10005.097</v>
+      </c>
+      <c r="J24" s="3">
+        <v>3016.1610000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>46502.530294138611</v>
       </c>
@@ -975,22 +1206,31 @@
         <v>14577</v>
       </c>
       <c r="C25">
-        <v>534.13484914188484</v>
+        <v>527.05639193848413</v>
       </c>
       <c r="D25">
-        <v>173.36419020798417</v>
+        <v>217.91126034786711</v>
       </c>
       <c r="E25">
-        <v>232.15290170360825</v>
+        <v>200.24473502092764</v>
       </c>
       <c r="F25">
-        <v>489.46581678993346</v>
+        <v>461.74981770787218</v>
       </c>
       <c r="G25" s="1">
         <v>32344</v>
       </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="H25" s="2">
+        <v>2190</v>
+      </c>
+      <c r="I25" s="3">
+        <v>9884.7240000000002</v>
+      </c>
+      <c r="J25" s="3">
+        <v>3035.8820000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>46645.570684873193</v>
       </c>
@@ -998,22 +1238,31 @@
         <v>14375</v>
       </c>
       <c r="C26">
-        <v>532.91103650907519</v>
+        <v>523.6692479855335</v>
       </c>
       <c r="D26">
-        <v>164.85382115122329</v>
+        <v>207.64155805215128</v>
       </c>
       <c r="E26">
-        <v>240.59481545141261</v>
+        <v>208.00923942389068</v>
       </c>
       <c r="F26">
-        <v>490.59182129474453</v>
+        <v>468.71543730523251</v>
       </c>
       <c r="G26" s="1">
         <v>32167</v>
       </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26" s="2">
+        <v>1937.7</v>
+      </c>
+      <c r="I26" s="3">
+        <v>9850.8320000000003</v>
+      </c>
+      <c r="J26" s="3">
+        <v>3040.5419999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>46724.291969960628</v>
       </c>
@@ -1021,22 +1270,31 @@
         <v>14355.6</v>
       </c>
       <c r="C27">
-        <v>528.74628783721664</v>
+        <v>525.24945865672248</v>
       </c>
       <c r="D27">
-        <v>162.93776083641859</v>
+        <v>205.78816499459583</v>
       </c>
       <c r="E27">
-        <v>233.44196653374627</v>
+        <v>208.08976816946327</v>
       </c>
       <c r="F27">
-        <v>498.18030899874844</v>
+        <v>469.80819699514427</v>
       </c>
       <c r="G27" s="1">
         <v>31957</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27" s="2">
+        <v>1820.5</v>
+      </c>
+      <c r="I27" s="3">
+        <v>9806.3770000000004</v>
+      </c>
+      <c r="J27" s="3">
+        <v>3096.0010000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>46773.028570150149</v>
       </c>
@@ -1044,22 +1302,31 @@
         <v>14402.5</v>
       </c>
       <c r="C28">
-        <v>528.62352290947399</v>
+        <v>517.16774736308344</v>
       </c>
       <c r="D28">
-        <v>163.54316824254025</v>
+        <v>211.67221307456788</v>
       </c>
       <c r="E28">
-        <v>249.91852088388987</v>
+        <v>206.72974389342107</v>
       </c>
       <c r="F28">
-        <v>482.23345275752064</v>
+        <v>459.83157484529431</v>
       </c>
       <c r="G28" s="1">
         <v>32076</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="H28" s="2">
+        <v>1804.7</v>
+      </c>
+      <c r="I28" s="3">
+        <v>9865.8639999999996</v>
+      </c>
+      <c r="J28" s="3">
+        <v>3112.9989999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>46817.391279722433</v>
       </c>
@@ -1067,22 +1334,31 @@
         <v>14541.9</v>
       </c>
       <c r="C29">
-        <v>532.51947937533748</v>
+        <v>518.92752913807215</v>
       </c>
       <c r="D29">
-        <v>169.89214951188706</v>
+        <v>213.0811033958507</v>
       </c>
       <c r="E29">
-        <v>240.11394485503746</v>
+        <v>201.46766234321328</v>
       </c>
       <c r="F29">
-        <v>486.20287501596954</v>
+        <v>466.56011611060023</v>
       </c>
       <c r="G29" s="1">
         <v>31999</v>
       </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="H29" s="2">
+        <v>1949.6</v>
+      </c>
+      <c r="I29" s="3">
+        <v>9864.8050000000003</v>
+      </c>
+      <c r="J29" s="3">
+        <v>3106.8220000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>46897.593140953424</v>
       </c>
@@ -1090,22 +1366,31 @@
         <v>14604.8</v>
       </c>
       <c r="C30">
-        <v>532.20698666337398</v>
+        <v>524.16360881091032</v>
       </c>
       <c r="D30">
-        <v>162.26906300151586</v>
+        <v>203.23374226785276</v>
       </c>
       <c r="E30">
-        <v>245.38478049063718</v>
+        <v>214.64539684103298</v>
       </c>
       <c r="F30">
-        <v>478.916729492939</v>
+        <v>454.0803215332607</v>
       </c>
       <c r="G30" s="1">
         <v>32106</v>
       </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="H30" s="2">
+        <v>2012.9</v>
+      </c>
+      <c r="I30" s="3">
+        <v>9917.6890000000003</v>
+      </c>
+      <c r="J30" s="3">
+        <v>3084.28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>46992.922439852846</v>
       </c>
@@ -1113,22 +1398,31 @@
         <v>14745.9</v>
       </c>
       <c r="C31">
-        <v>528.7625565736156</v>
+        <v>519.60735789148794</v>
       </c>
       <c r="D31">
-        <v>167.71200270290737</v>
+        <v>205.38048921061181</v>
       </c>
       <c r="E31">
-        <v>232.56347710283313</v>
+        <v>198.76925205071075</v>
       </c>
       <c r="F31">
-        <v>496.16486914411519</v>
+        <v>482.18361053333433</v>
       </c>
       <c r="G31" s="1">
         <v>32308</v>
       </c>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="H31" s="2">
+        <v>2116.9</v>
+      </c>
+      <c r="I31" s="3">
+        <v>9998.3889999999992</v>
+      </c>
+      <c r="J31" s="3">
+        <v>3106.2089999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>47113.422604278494</v>
       </c>
@@ -1136,22 +1430,31 @@
         <v>14845.5</v>
       </c>
       <c r="C32">
-        <v>530.68947744224567</v>
+        <v>517.9105697416187</v>
       </c>
       <c r="D32">
-        <v>171.52866526434701</v>
+        <v>211.39713982338247</v>
       </c>
       <c r="E32">
-        <v>239.78312238728091</v>
+        <v>206.58138537053912</v>
       </c>
       <c r="F32">
-        <v>479.47388062317395</v>
+        <v>456.11528989005677</v>
       </c>
       <c r="G32" s="1">
         <v>32452</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32" s="2">
+        <v>2185.6999999999998</v>
+      </c>
+      <c r="I32" s="3">
+        <v>10063.083000000001</v>
+      </c>
+      <c r="J32" s="3">
+        <v>3103.5329999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>47250.074708542437</v>
       </c>
@@ -1159,22 +1462,31 @@
         <v>14939</v>
       </c>
       <c r="C33">
-        <v>536.07193116387077</v>
+        <v>522.58175502044901</v>
       </c>
       <c r="D33">
-        <v>163.84389987263785</v>
+        <v>206.96009294155809</v>
       </c>
       <c r="E33">
-        <v>228.16103674361023</v>
+        <v>190.77828593580153</v>
       </c>
       <c r="F33">
-        <v>488.80395691341232</v>
+        <v>469.25772490487878</v>
       </c>
       <c r="G33" s="1">
         <v>32718</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33" s="2">
+        <v>2166.1</v>
+      </c>
+      <c r="I33" s="3">
+        <v>10166.127</v>
+      </c>
+      <c r="J33" s="3">
+        <v>3071.5239999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34">
         <v>47380.638269809984</v>
       </c>
@@ -1182,22 +1494,31 @@
         <v>14881.3</v>
       </c>
       <c r="C34">
-        <v>528.63381197100239</v>
+        <v>520.84708278519997</v>
       </c>
       <c r="D34">
-        <v>166.96292714618039</v>
+        <v>206.3848147040639</v>
       </c>
       <c r="E34">
-        <v>238.33931949962451</v>
+        <v>205.20981759144667</v>
       </c>
       <c r="F34">
-        <v>491.84592393349203</v>
+        <v>468.43948212469536</v>
       </c>
       <c r="G34" s="1">
         <v>32827</v>
       </c>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="H34" s="2">
+        <v>2125.9</v>
+      </c>
+      <c r="I34" s="3">
+        <v>10217.123</v>
+      </c>
+      <c r="J34" s="3">
+        <v>3012.2159999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>47500.016243688187</v>
       </c>
@@ -1205,22 +1526,31 @@
         <v>14989.6</v>
       </c>
       <c r="C35">
-        <v>529.5415134638688</v>
+        <v>520.90650060971552</v>
       </c>
       <c r="D35">
-        <v>166.92736730950324</v>
+        <v>205.05606261204119</v>
       </c>
       <c r="E35">
-        <v>234.36860896604031</v>
+        <v>206.89105537798076</v>
       </c>
       <c r="F35">
-        <v>493.91363999508224</v>
+        <v>471.91303676552184</v>
       </c>
       <c r="G35" s="1">
         <v>32838</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="H35" s="2">
+        <v>2208</v>
+      </c>
+      <c r="I35" s="3">
+        <v>10237.675999999999</v>
+      </c>
+      <c r="J35" s="3">
+        <v>3008.9949999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36">
         <v>47638.880917749921</v>
       </c>
@@ -1228,22 +1558,31 @@
         <v>15021.1</v>
       </c>
       <c r="C36">
-        <v>534.66563228811515</v>
+        <v>528.50057786323498</v>
       </c>
       <c r="D36">
-        <v>170.11001464321296</v>
+        <v>210.36650762510527</v>
       </c>
       <c r="E36">
-        <v>235.84636781835434</v>
+        <v>197.68168431964338</v>
       </c>
       <c r="F36">
-        <v>484.87533316032199</v>
+        <v>459.90816840205002</v>
       </c>
       <c r="G36" s="1">
         <v>32915</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="H36" s="2">
+        <v>2214</v>
+      </c>
+      <c r="I36" s="3">
+        <v>10282.234</v>
+      </c>
+      <c r="J36" s="3">
+        <v>2990.0059999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37">
         <v>47778.037804806161</v>
       </c>
@@ -1251,22 +1590,31 @@
         <v>15190.3</v>
       </c>
       <c r="C37">
-        <v>535.4915787559861</v>
+        <v>526.55143067690415</v>
       </c>
       <c r="D37">
-        <v>174.47787570744325</v>
+        <v>217.18399667558967</v>
       </c>
       <c r="E37">
-        <v>225.44193040541998</v>
+        <v>187.11597502830909</v>
       </c>
       <c r="F37">
-        <v>488.72513422542283</v>
+        <v>465.28726413281618</v>
       </c>
       <c r="G37" s="1">
         <v>32961</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="H37" s="2">
+        <v>2373.6999999999998</v>
+      </c>
+      <c r="I37" s="3">
+        <v>10316.777</v>
+      </c>
+      <c r="J37" s="3">
+        <v>2978.279</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38">
         <v>47955.909363310187</v>
       </c>
@@ -1274,22 +1622,31 @@
         <v>15291</v>
       </c>
       <c r="C38">
-        <v>529.32189147544852</v>
+        <v>525.18318650167294</v>
       </c>
       <c r="D38">
-        <v>172.05660864988303</v>
+        <v>216.54872993421677</v>
       </c>
       <c r="E38">
-        <v>229.3866826491531</v>
+        <v>189.54133545142884</v>
       </c>
       <c r="F38">
-        <v>497.03988762728193</v>
+        <v>472.0698303190199</v>
       </c>
       <c r="G38" s="1">
         <v>33105</v>
       </c>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="H38" s="2">
+        <v>2429.6</v>
+      </c>
+      <c r="I38" s="3">
+        <v>10379.022000000001</v>
+      </c>
+      <c r="J38" s="3">
+        <v>2963.7139999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39">
         <v>48146.208869200156</v>
       </c>
@@ -1297,22 +1654,31 @@
         <v>15362.4</v>
       </c>
       <c r="C39">
-        <v>530.56220474179008</v>
+        <v>519.33654199195325</v>
       </c>
       <c r="D39">
-        <v>168.64095557740836</v>
+        <v>212.02039261008767</v>
       </c>
       <c r="E39">
-        <v>227.32628315697002</v>
+        <v>196.25655538383103</v>
       </c>
       <c r="F39">
-        <v>501.39665762052203</v>
+        <v>481.72653957437421</v>
       </c>
       <c r="G39" s="1">
         <v>33106</v>
       </c>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="H39" s="2">
+        <v>2489.1</v>
+      </c>
+      <c r="I39" s="3">
+        <v>10396.629999999999</v>
+      </c>
+      <c r="J39" s="3">
+        <v>2949.3780000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40">
         <v>48349.728229374203</v>
       </c>
@@ -1320,22 +1686,31 @@
         <v>15380.8</v>
       </c>
       <c r="C40">
-        <v>527.90196452354701</v>
+        <v>520.04533629259925</v>
       </c>
       <c r="D40">
-        <v>165.67715147610116</v>
+        <v>210.29844017863385</v>
       </c>
       <c r="E40">
-        <v>239.05374665362945</v>
+        <v>198.49297438151203</v>
       </c>
       <c r="F40">
-        <v>496.03249899453772</v>
+        <v>468.5771858547036</v>
       </c>
       <c r="G40" s="1">
         <v>33128</v>
       </c>
-    </row>
-    <row r="41" spans="1:7">
+      <c r="H40" s="2">
+        <v>2482</v>
+      </c>
+      <c r="I40" s="3">
+        <v>10424.119000000001</v>
+      </c>
+      <c r="J40" s="3">
+        <v>2940.8560000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41">
         <v>48549.702463054629</v>
       </c>
@@ -1343,22 +1718,31 @@
         <v>15384.3</v>
       </c>
       <c r="C41">
-        <v>542.63136780423042</v>
+        <v>532.49196688810332</v>
       </c>
       <c r="D41">
-        <v>161.58571726448329</v>
+        <v>209.44029141087785</v>
       </c>
       <c r="E41">
-        <v>232.19474050758106</v>
+        <v>195.10264442083133</v>
       </c>
       <c r="F41">
-        <v>491.43338550348921</v>
+        <v>461.15150511052309</v>
       </c>
       <c r="G41" s="1">
         <v>33156</v>
       </c>
-    </row>
-    <row r="42" spans="1:7">
+      <c r="H41" s="2">
+        <v>2462.1999999999998</v>
+      </c>
+      <c r="I41" s="3">
+        <v>10453.204</v>
+      </c>
+      <c r="J41" s="3">
+        <v>2912.2689999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42">
         <v>48742.987404272782</v>
       </c>
@@ -1366,22 +1750,31 @@
         <v>15491.9</v>
       </c>
       <c r="C42">
-        <v>528.67911824804821</v>
+        <v>522.73118809982452</v>
       </c>
       <c r="D42">
-        <v>170.11330275136334</v>
+        <v>210.04324576368964</v>
       </c>
       <c r="E42">
-        <v>232.37414808314992</v>
+        <v>202.38518993776353</v>
       </c>
       <c r="F42">
-        <v>496.08840229912988</v>
+        <v>469.10527849354446</v>
       </c>
       <c r="G42" s="1">
         <v>33261</v>
       </c>
-    </row>
-    <row r="43" spans="1:7">
+      <c r="H42" s="2">
+        <v>2543</v>
+      </c>
+      <c r="I42" s="3">
+        <v>10502.3</v>
+      </c>
+      <c r="J42" s="3">
+        <v>2880.5740000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43">
         <v>48954.791233703945</v>
       </c>
@@ -1389,22 +1782,31 @@
         <v>15521.6</v>
       </c>
       <c r="C43">
-        <v>527.84207537918974</v>
+        <v>527.48401203628543</v>
       </c>
       <c r="D43">
-        <v>158.51115186686039</v>
+        <v>202.08928292952561</v>
       </c>
       <c r="E43">
-        <v>228.86551479540179</v>
+        <v>201.39226175452251</v>
       </c>
       <c r="F43">
-        <v>503.46081995278212</v>
+        <v>469.62271094376132</v>
       </c>
       <c r="G43" s="1">
         <v>33277</v>
       </c>
-    </row>
-    <row r="44" spans="1:7">
+      <c r="H43" s="2">
+        <v>2574.3000000000002</v>
+      </c>
+      <c r="I43" s="3">
+        <v>10523.929</v>
+      </c>
+      <c r="J43" s="3">
+        <v>2866.2310000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44">
         <v>49172.57788178388</v>
       </c>
@@ -1412,22 +1814,31 @@
         <v>15641.3</v>
       </c>
       <c r="C44">
-        <v>532.26097558279184</v>
+        <v>522.36998553201352</v>
       </c>
       <c r="D44">
-        <v>168.07252744223797</v>
+        <v>206.67942350246571</v>
       </c>
       <c r="E44">
-        <v>235.57174673386595</v>
+        <v>199.35540208599491</v>
       </c>
       <c r="F44">
-        <v>483.92083534453388</v>
+        <v>458.85565278262396</v>
       </c>
       <c r="G44" s="1">
         <v>33367</v>
       </c>
-    </row>
-    <row r="45" spans="1:7">
+      <c r="H44" s="2">
+        <v>2656.8</v>
+      </c>
+      <c r="I44" s="3">
+        <v>10573.135</v>
+      </c>
+      <c r="J44" s="3">
+        <v>2851.9549999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45">
         <v>49409.095312451806</v>
       </c>
@@ -1435,22 +1846,31 @@
         <v>15793.9</v>
       </c>
       <c r="C45">
-        <v>536.96220976530765</v>
+        <v>527.0569623485427</v>
       </c>
       <c r="D45">
-        <v>169.65793627673338</v>
+        <v>208.21685669680306</v>
       </c>
       <c r="E45">
-        <v>231.70007261029443</v>
+        <v>197.75748404326401</v>
       </c>
       <c r="F45">
-        <v>490.33936698037917</v>
+        <v>467.39567446088699</v>
       </c>
       <c r="G45" s="1">
         <v>33580</v>
       </c>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="H45" s="2">
+        <v>2692</v>
+      </c>
+      <c r="I45" s="3">
+        <v>10662.222</v>
+      </c>
+      <c r="J45" s="3">
+        <v>2831.451</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46">
         <v>49652.355613174608</v>
       </c>
@@ -1458,22 +1878,31 @@
         <v>15757.6</v>
       </c>
       <c r="C46">
-        <v>533.67300307386301</v>
+        <v>530.44410218302528</v>
       </c>
       <c r="D46">
-        <v>170.22024837923584</v>
+        <v>216.1192917169991</v>
       </c>
       <c r="E46">
-        <v>234.39002045445272</v>
+        <v>205.21425534133931</v>
       </c>
       <c r="F46">
-        <v>488.5157921222692</v>
+        <v>455.92019252666387</v>
       </c>
       <c r="G46" s="1">
         <v>33684</v>
       </c>
-    </row>
-    <row r="47" spans="1:7">
+      <c r="H46" s="2">
+        <v>2652.5</v>
+      </c>
+      <c r="I46" s="3">
+        <v>10713.384</v>
+      </c>
+      <c r="J46" s="3">
+        <v>2827.201</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47">
         <v>49883.625137281429</v>
       </c>
@@ -1481,22 +1910,31 @@
         <v>15935.8</v>
       </c>
       <c r="C47">
-        <v>528.82856412336218</v>
+        <v>522.58024890195816</v>
       </c>
       <c r="D47">
-        <v>172.66435911782503</v>
+        <v>214.49900240487273</v>
       </c>
       <c r="E47">
-        <v>231.49168073802218</v>
+        <v>203.1857235414987</v>
       </c>
       <c r="F47">
-        <v>495.75394981122713</v>
+        <v>473.39842864899902</v>
       </c>
       <c r="G47" s="1">
         <v>33915</v>
       </c>
-    </row>
-    <row r="48" spans="1:7">
+      <c r="H47" s="2">
+        <v>2750.6</v>
+      </c>
+      <c r="I47" s="3">
+        <v>10805.115</v>
+      </c>
+      <c r="J47" s="3">
+        <v>2834.6680000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48">
         <v>50137.408175545148</v>
       </c>
@@ -1504,22 +1942,31 @@
         <v>16139.5</v>
       </c>
       <c r="C48">
-        <v>537.53768707814038</v>
+        <v>531.9442578732594</v>
       </c>
       <c r="D48">
-        <v>170.9979103312339</v>
+        <v>216.58788067921233</v>
       </c>
       <c r="E48">
-        <v>234.12626145842145</v>
+        <v>195.59824722968858</v>
       </c>
       <c r="F48">
-        <v>487.21736709905474</v>
+        <v>460.08450906400674</v>
       </c>
       <c r="G48" s="1">
         <v>34173</v>
       </c>
-    </row>
-    <row r="49" spans="1:7">
+      <c r="H48" s="2">
+        <v>2826.4</v>
+      </c>
+      <c r="I48" s="3">
+        <v>10909.861999999999</v>
+      </c>
+      <c r="J48" s="3">
+        <v>2849.5070000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49">
         <v>50407.933914811474</v>
       </c>
@@ -1527,22 +1974,31 @@
         <v>16220.2</v>
       </c>
       <c r="C49">
-        <v>535.80173743170963</v>
+        <v>529.03307879998829</v>
       </c>
       <c r="D49">
-        <v>171.15246712231038</v>
+        <v>209.97078575582577</v>
       </c>
       <c r="E49">
-        <v>229.0804666567137</v>
+        <v>193.26683992316271</v>
       </c>
       <c r="F49">
-        <v>489.37591043301688</v>
+        <v>466.05136670598654</v>
       </c>
       <c r="G49" s="1">
         <v>34526</v>
       </c>
-    </row>
-    <row r="50" spans="1:7">
+      <c r="H49" s="2">
+        <v>2817.3</v>
+      </c>
+      <c r="I49" s="3">
+        <v>11045.225</v>
+      </c>
+      <c r="J49" s="3">
+        <v>2845.038</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50">
         <v>50673.831734051557</v>
       </c>
@@ -1550,22 +2006,31 @@
         <v>16350</v>
       </c>
       <c r="C50">
-        <v>533.64192394273437</v>
+        <v>530.13818868547139</v>
       </c>
       <c r="D50">
-        <v>166.45958457109998</v>
+        <v>214.04912295640875</v>
       </c>
       <c r="E50">
-        <v>241.07324761844967</v>
+        <v>204.50049494361224</v>
       </c>
       <c r="F50">
-        <v>489.17586357427024</v>
+        <v>463.29197504745468</v>
       </c>
       <c r="G50" s="1">
         <v>34782</v>
       </c>
-    </row>
-    <row r="51" spans="1:7">
+      <c r="H50" s="2">
+        <v>2905.4</v>
+      </c>
+      <c r="I50" s="3">
+        <v>11145.286</v>
+      </c>
+      <c r="J50" s="3">
+        <v>2855.7260000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51">
         <v>50959.441884983185</v>
       </c>
@@ -1573,22 +2038,31 @@
         <v>16460.900000000001</v>
       </c>
       <c r="C51">
-        <v>533.18431244132</v>
+        <v>528.8993913209772</v>
       </c>
       <c r="D51">
-        <v>171.80134892928564</v>
+        <v>219.17407101173461</v>
       </c>
       <c r="E51">
-        <v>226.26445505511947</v>
+        <v>198.8154555450285</v>
       </c>
       <c r="F51">
-        <v>497.41126643654309</v>
+        <v>464.98957500809712</v>
       </c>
       <c r="G51" s="1">
         <v>34981</v>
       </c>
-    </row>
-    <row r="52" spans="1:7">
+      <c r="H51" s="2">
+        <v>2911.3</v>
+      </c>
+      <c r="I51" s="3">
+        <v>11227.947</v>
+      </c>
+      <c r="J51" s="3">
+        <v>2879.8850000000002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52">
         <v>51244.042917968596</v>
       </c>
@@ -1596,22 +2070,31 @@
         <v>16527.599999999999</v>
       </c>
       <c r="C52">
-        <v>537.93646994787537</v>
+        <v>532.82087895549273</v>
       </c>
       <c r="D52">
-        <v>164.89418121276901</v>
+        <v>203.96742703817915</v>
       </c>
       <c r="E52">
-        <v>243.19869865984356</v>
+        <v>209.0208112788479</v>
       </c>
       <c r="F52">
-        <v>482.70378305555266</v>
+        <v>454.88534958062246</v>
       </c>
       <c r="G52" s="1">
         <v>35149</v>
       </c>
-    </row>
-    <row r="53" spans="1:7">
+      <c r="H52" s="2">
+        <v>2925.5</v>
+      </c>
+      <c r="I52" s="3">
+        <v>11304.566999999999</v>
+      </c>
+      <c r="J52" s="3">
+        <v>2888.2510000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53">
         <v>51529.718609894728</v>
       </c>
@@ -1619,22 +2102,31 @@
         <v>16547.599999999999</v>
       </c>
       <c r="C53">
-        <v>534.38528482862057</v>
+        <v>530.34208875825846</v>
       </c>
       <c r="D53">
-        <v>170.80346291883274</v>
+        <v>212.79167391098571</v>
       </c>
       <c r="E53">
-        <v>236.30154770772543</v>
+        <v>199.21746908473361</v>
       </c>
       <c r="F53">
-        <v>489.4094911273595</v>
+        <v>462.76090300979604</v>
       </c>
       <c r="G53" s="1">
         <v>35310</v>
       </c>
-    </row>
-    <row r="54" spans="1:7">
+      <c r="H53" s="2">
+        <v>2879.2</v>
+      </c>
+      <c r="I53" s="3">
+        <v>11379.272999999999</v>
+      </c>
+      <c r="J53" s="3">
+        <v>2890.2379999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54">
         <v>51801.334613826417</v>
       </c>
@@ -1642,22 +2134,31 @@
         <v>16571.599999999999</v>
       </c>
       <c r="C54">
-        <v>534.00740126717994</v>
+        <v>531.0995666412889</v>
       </c>
       <c r="D54">
-        <v>179.48980407471666</v>
+        <v>220.24463510981437</v>
       </c>
       <c r="E54">
-        <v>242.58719969251928</v>
+        <v>213.40577807978605</v>
       </c>
       <c r="F54">
-        <v>476.50888848218506</v>
+        <v>446.61236487076872</v>
       </c>
       <c r="G54" s="1">
         <v>35411</v>
       </c>
-    </row>
-    <row r="55" spans="1:7">
+      <c r="H54" s="2">
+        <v>2849.8</v>
+      </c>
+      <c r="I54" s="3">
+        <v>11430.549000000001</v>
+      </c>
+      <c r="J54" s="3">
+        <v>2903.1869999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55">
         <v>52063.238215064623</v>
       </c>
@@ -1665,22 +2166,31 @@
         <v>16663.5</v>
       </c>
       <c r="C55">
-        <v>533.8938686613476</v>
+        <v>529.33792713586831</v>
       </c>
       <c r="D55">
-        <v>168.56622155523132</v>
+        <v>213.38404703745209</v>
       </c>
       <c r="E55">
-        <v>233.13952757325916</v>
+        <v>204.28637429548544</v>
       </c>
       <c r="F55">
-        <v>491.91669028949059</v>
+        <v>461.47144664714773</v>
       </c>
       <c r="G55" s="1">
         <v>35685</v>
       </c>
-    </row>
-    <row r="56" spans="1:7">
+      <c r="H55" s="2">
+        <v>2830.2</v>
+      </c>
+      <c r="I55" s="3">
+        <v>11537.727999999999</v>
+      </c>
+      <c r="J55" s="3">
+        <v>2896.3319999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56">
         <v>52317.963888036305</v>
       </c>
@@ -1688,22 +2198,31 @@
         <v>16778.099999999999</v>
       </c>
       <c r="C56">
-        <v>533.375409024992</v>
+        <v>525.90458767927657</v>
       </c>
       <c r="D56">
-        <v>174.5728136018146</v>
+        <v>212.18384304436947</v>
       </c>
       <c r="E56">
-        <v>234.38962512880585</v>
+        <v>204.91915638851702</v>
       </c>
       <c r="F56">
-        <v>482.3464547322763</v>
+        <v>453.51143316009825</v>
       </c>
       <c r="G56" s="1">
         <v>35863</v>
       </c>
-    </row>
-    <row r="57" spans="1:7">
+      <c r="H56" s="2">
+        <v>2847.2</v>
+      </c>
+      <c r="I56" s="3">
+        <v>11618.098</v>
+      </c>
+      <c r="J56" s="3">
+        <v>2899.9360000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57">
         <v>52574.724063367146</v>
       </c>
@@ -1711,32 +2230,51 @@
         <v>16851.400000000001</v>
       </c>
       <c r="C57">
-        <v>536.31063867641069</v>
+        <v>524.3100530034277</v>
       </c>
       <c r="D57">
-        <v>172.05002411065698</v>
+        <v>220.52043639767265</v>
       </c>
       <c r="E57">
-        <v>235.5783258264201</v>
+        <v>201.57270661780262</v>
       </c>
       <c r="F57">
-        <v>486.78737095381598</v>
+        <v>457.72846912167495</v>
       </c>
       <c r="G57" s="1">
         <v>36052</v>
       </c>
-    </row>
-    <row r="58" spans="1:7">
+      <c r="H57" s="2">
+        <v>2905.7</v>
+      </c>
+      <c r="I57" s="3">
+        <v>11702.12</v>
+      </c>
+      <c r="J57" s="3">
+        <v>2901.1840000000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="G58" s="1"/>
-    </row>
-    <row r="59" spans="1:7">
+      <c r="H58" s="2"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+    </row>
+    <row r="59" spans="1:10">
       <c r="G59" s="1"/>
-    </row>
-    <row r="60" spans="1:7">
+      <c r="H59" s="2"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+    </row>
+    <row r="60" spans="1:10">
       <c r="G60" s="1"/>
-    </row>
-    <row r="61" spans="1:7">
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+    </row>
+    <row r="61" spans="1:10">
       <c r="G61" s="1"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>